<commit_message>
add count macrofauna composition analysis
</commit_message>
<xml_diff>
--- a/table/count_permanova.xlsx
+++ b/table/count_permanova.xlsx
@@ -390,44 +390,44 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.4589251995768713</v>
+        <v>0.3783812185883571</v>
       </c>
       <c r="C2">
-        <v>0.04106381961039329</v>
+        <v>0.05841353132863106</v>
       </c>
       <c r="D2">
-        <v>1.716092978507632</v>
+        <v>2.731812415818474</v>
       </c>
       <c r="E2">
-        <v>0.04554</v>
+        <v>0.0043</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>4.031365273707566</v>
+        <v>3.052045430404583</v>
       </c>
       <c r="C3">
-        <v>0.3607194735346022</v>
+        <v>0.4711670204733284</v>
       </c>
       <c r="D3">
-        <v>2.512463776372717</v>
+        <v>2.448329060401857</v>
       </c>
       <c r="E3">
-        <v>1e-005</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>6.685610938982555</v>
+        <v>3.047202934118666</v>
       </c>
       <c r="C4">
-        <v>0.5982167068550047</v>
+        <v>0.4704194481980408</v>
       </c>
     </row>
     <row r="5">
@@ -435,7 +435,7 @@
         <v>32</v>
       </c>
       <c r="B5">
-        <v>11.17590141226699</v>
+        <v>6.477629583111605</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -491,19 +491,19 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.04166321318293622</v>
+        <v>0.00345141700045872</v>
       </c>
       <c r="C2">
-        <v>0.04166321318293622</v>
+        <v>0.00345141700045872</v>
       </c>
       <c r="D2">
-        <v>5.747000106313553</v>
+        <v>0.3673203149951823</v>
       </c>
       <c r="E2">
         <v>999</v>
       </c>
       <c r="F2">
-        <v>0.032</v>
+        <v>0.546</v>
       </c>
     </row>
     <row r="3">
@@ -511,10 +511,10 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>0.2247363119503231</v>
+        <v>0.2912823566962901</v>
       </c>
       <c r="C3">
-        <v>0.007249558450010424</v>
+        <v>0.009396205054719034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>